<commit_message>
agregado de numeros aguja y brazuelo
</commit_message>
<xml_diff>
--- a/Copia de Codigos CHABAT.xlsx
+++ b/Copia de Codigos CHABAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA22B6C-6014-4CC8-983D-E4B5ADD7E358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159660F5-ABFA-44D2-93EC-B9FBF1AA2961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1195,6 +1195,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1230,27 +1251,6 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1547,7 +1547,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1583,68 +1583,68 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="88" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="86" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="85" t="s">
+      <c r="J2" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="84" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="87"/>
+      <c r="M2" s="75"/>
       <c r="P2" s="67">
         <v>45555</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="82"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="9" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="76"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="78"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="77" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="88" t="s">
+      <c r="N3" s="76" t="s">
         <v>189</v>
       </c>
       <c r="P3" s="4" t="s">
@@ -1688,8 +1688,8 @@
       <c r="L4" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="90"/>
-      <c r="N4" s="88">
+      <c r="M4" s="78"/>
+      <c r="N4" s="76">
         <v>171</v>
       </c>
       <c r="P4" s="68" t="s">
@@ -1733,8 +1733,8 @@
       <c r="L5" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="90"/>
-      <c r="N5" s="88">
+      <c r="M5" s="78"/>
+      <c r="N5" s="76">
         <v>170</v>
       </c>
     </row>
@@ -1771,8 +1771,8 @@
       <c r="L6" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="90"/>
-      <c r="N6" s="88" t="s">
+      <c r="M6" s="78"/>
+      <c r="N6" s="76" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1813,8 +1813,8 @@
       <c r="L7" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="90"/>
-      <c r="N7" s="88" t="s">
+      <c r="M7" s="78"/>
+      <c r="N7" s="76" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1853,8 +1853,10 @@
       <c r="L8" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="90"/>
-      <c r="N8" s="88" t="s">
+      <c r="M8" s="78">
+        <v>100</v>
+      </c>
+      <c r="N8" s="76" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1895,8 +1897,8 @@
       <c r="L9" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="90"/>
-      <c r="N9" s="88" t="s">
+      <c r="M9" s="78"/>
+      <c r="N9" s="76" t="s">
         <v>190</v>
       </c>
     </row>
@@ -1937,8 +1939,8 @@
       <c r="L10" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="91"/>
-      <c r="N10" s="88">
+      <c r="M10" s="79"/>
+      <c r="N10" s="76">
         <v>130</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -1982,8 +1984,8 @@
       <c r="L11" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M11" s="90"/>
-      <c r="N11" s="88"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="76"/>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
@@ -2022,8 +2024,8 @@
       <c r="L12" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="91"/>
-      <c r="N12" s="88">
+      <c r="M12" s="79"/>
+      <c r="N12" s="76">
         <v>172</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -2067,8 +2069,8 @@
       <c r="L13" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M13" s="90"/>
-      <c r="N13" s="88"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="76"/>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
@@ -2107,8 +2109,8 @@
       <c r="L14" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M14" s="90"/>
-      <c r="N14" s="88"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="76"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
@@ -2147,8 +2149,8 @@
       <c r="L15" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M15" s="91"/>
-      <c r="N15" s="88"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="76"/>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
@@ -2185,8 +2187,8 @@
       <c r="L16" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="90"/>
-      <c r="N16" s="88"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="76"/>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
@@ -2223,8 +2225,8 @@
       <c r="L17" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="90"/>
-      <c r="N17" s="88"/>
+      <c r="M17" s="78"/>
+      <c r="N17" s="76"/>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
@@ -2263,8 +2265,8 @@
       <c r="L18" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="91"/>
-      <c r="N18" s="88"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="76"/>
     </row>
     <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
@@ -2301,10 +2303,10 @@
       <c r="L19" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="90">
+      <c r="M19" s="78">
         <v>101</v>
       </c>
-      <c r="N19" s="88"/>
+      <c r="N19" s="76"/>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
@@ -2341,8 +2343,8 @@
       <c r="L20" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="90"/>
-      <c r="N20" s="88"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="76"/>
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -2379,8 +2381,8 @@
       <c r="L21" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="90"/>
-      <c r="N21" s="88"/>
+      <c r="M21" s="78"/>
+      <c r="N21" s="76"/>
     </row>
     <row r="22" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
@@ -2419,8 +2421,10 @@
       <c r="L22" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M22" s="90"/>
-      <c r="N22" s="88"/>
+      <c r="M22" s="78">
+        <v>103</v>
+      </c>
+      <c r="N22" s="76"/>
     </row>
     <row r="23" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
@@ -2455,8 +2459,8 @@
       <c r="L23" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M23" s="90"/>
-      <c r="N23" s="88"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="76"/>
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
@@ -2495,8 +2499,8 @@
       <c r="L24" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M24" s="90"/>
-      <c r="N24" s="88"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="76"/>
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
@@ -2535,8 +2539,8 @@
       <c r="L25" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="M25" s="90"/>
-      <c r="N25" s="88"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="76"/>
     </row>
     <row r="26" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
@@ -2575,8 +2579,8 @@
       <c r="L26" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M26" s="90"/>
-      <c r="N26" s="88"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="76"/>
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -2613,8 +2617,8 @@
       <c r="L27" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M27" s="90"/>
-      <c r="N27" s="88"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="76"/>
     </row>
     <row r="28" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
@@ -2653,8 +2657,8 @@
       <c r="L28" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M28" s="90"/>
-      <c r="N28" s="88"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="76"/>
     </row>
     <row r="29" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
@@ -2691,8 +2695,8 @@
       <c r="L29" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="90"/>
-      <c r="N29" s="88"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="76"/>
     </row>
     <row r="30" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
@@ -2727,8 +2731,8 @@
       <c r="L30" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M30" s="90"/>
-      <c r="N30" s="88"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="76"/>
     </row>
     <row r="31" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
@@ -2763,8 +2767,8 @@
       <c r="L31" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M31" s="90"/>
-      <c r="N31" s="88"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="76"/>
     </row>
     <row r="32" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
@@ -2801,8 +2805,8 @@
       <c r="L32" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M32" s="90"/>
-      <c r="N32" s="88"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="76"/>
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
@@ -2835,8 +2839,8 @@
       <c r="L33" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M33" s="90"/>
-      <c r="N33" s="88"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="76"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
@@ -2871,8 +2875,8 @@
       <c r="L34" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="90"/>
-      <c r="N34" s="88"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="76"/>
     </row>
     <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
@@ -2907,8 +2911,8 @@
       <c r="L35" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="M35" s="92"/>
-      <c r="N35" s="88"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="76"/>
     </row>
     <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
@@ -2943,8 +2947,8 @@
       <c r="L36" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="M36" s="92"/>
-      <c r="N36" s="88"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="76"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
@@ -2981,8 +2985,8 @@
       <c r="L37" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="M37" s="92"/>
-      <c r="N37" s="88"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="76"/>
     </row>
     <row r="38" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="33"/>
@@ -3019,8 +3023,8 @@
       <c r="L38" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="M38" s="93"/>
-      <c r="N38" s="88"/>
+      <c r="M38" s="81"/>
+      <c r="N38" s="76"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="38"/>
@@ -3117,6 +3121,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100E111FB68E4AB3A458E6F1E68F8888CED" ma:contentTypeVersion="13" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="bfe1cfa8ea064de69b4e2203b8e1e509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4613b05c-4671-4207-a6b8-e30994dce502" xmlns:ns3="ae89acfa-0242-4570-84ca-e3aafb74daca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b8d078cf0bd54969afc6a4d318ee940" ns2:_="" ns3:_="">
     <xsd:import namespace="4613b05c-4671-4207-a6b8-e30994dce502"/>
@@ -3339,15 +3352,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3360,6 +3364,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A9BCE7-9EE4-4695-9AF6-872741DC1E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3378,14 +3390,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C716C4-15E6-42BB-B1FF-483DC7FD91F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B61C396E-4544-457B-B310-CE821083C357}">
   <ds:schemaRefs>

</xml_diff>